<commit_message>
úprava tabulky pro charakter
</commit_message>
<xml_diff>
--- a/Public/tabulka-charakteru.xlsx
+++ b/Public/tabulka-charakteru.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="150" yWindow="570" windowWidth="28455" windowHeight="11955"/>
+    <workbookView xWindow="240" yWindow="495" windowWidth="19815" windowHeight="4815"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
   <si>
     <t>lel</t>
   </si>
@@ -37,9 +37,6 @@
   </si>
   <si>
     <t>Původ</t>
-  </si>
-  <si>
-    <t>Náboženství (pokuď)</t>
   </si>
   <si>
     <t>Věk</t>
@@ -81,9 +78,6 @@
     <t>Síla</t>
   </si>
   <si>
-    <t>Detství</t>
-  </si>
-  <si>
     <t>Obratnost</t>
   </si>
   <si>
@@ -108,6 +102,9 @@
     <t>2.</t>
   </si>
   <si>
+    <t>Dětství</t>
+  </si>
+  <si>
     <t>Vitalita</t>
   </si>
 </sst>
@@ -115,7 +112,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -135,6 +132,13 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -144,12 +148,23 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -167,42 +182,22 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -213,17 +208,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="normální" xfId="0" builtinId="0"/>
@@ -518,27 +511,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y1000"/>
+  <dimension ref="A1:AA1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U29" sqref="T29:U29"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="3" width="7.5703125" customWidth="1"/>
     <col min="4" max="4" width="13.42578125" customWidth="1"/>
-    <col min="5" max="6" width="7.5703125" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" customWidth="1"/>
+    <col min="5" max="7" width="7.5703125" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" customWidth="1"/>
     <col min="9" max="10" width="7.5703125" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" customWidth="1"/>
+    <col min="11" max="11" width="8.7109375" customWidth="1"/>
     <col min="12" max="12" width="7.42578125" customWidth="1"/>
     <col min="13" max="13" width="9.140625" customWidth="1"/>
-    <col min="14" max="26" width="7.5703125" customWidth="1"/>
+    <col min="14" max="15" width="7.5703125" customWidth="1"/>
+    <col min="16" max="16" width="10.28515625" customWidth="1"/>
+    <col min="17" max="26" width="7.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:27">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -546,545 +540,768 @@
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="1:25">
-      <c r="D2" s="3" t="s">
+    <row r="2" spans="1:27">
+      <c r="D2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
-      <c r="O2" s="5" t="s">
+      <c r="O2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="P2" s="4"/>
-    </row>
-    <row r="3" spans="1:25">
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
+      <c r="P2" s="9"/>
+    </row>
+    <row r="3" spans="1:27">
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-    </row>
-    <row r="4" spans="1:25">
-      <c r="D4" s="1" t="s">
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+    </row>
+    <row r="4" spans="1:27">
+      <c r="D4" s="16" t="s">
         <v>3</v>
       </c>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
-      <c r="O4" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25">
+    </row>
+    <row r="5" spans="1:27">
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
-      <c r="P5" s="1" t="s">
+      <c r="O5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27">
+      <c r="D6" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="R5" s="11"/>
-      <c r="S5" s="11"/>
-      <c r="T5" s="11"/>
-      <c r="U5" s="11"/>
-      <c r="V5" s="11"/>
-      <c r="W5" s="11"/>
-      <c r="X5" s="11"/>
-      <c r="Y5" s="11"/>
-    </row>
-    <row r="6" spans="1:25">
-      <c r="D6" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
+      <c r="O6" s="3"/>
       <c r="P6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
-      <c r="R6" s="11"/>
-      <c r="S6" s="11"/>
-      <c r="T6" s="11"/>
-      <c r="U6" s="11"/>
-      <c r="V6" s="11"/>
-      <c r="W6" s="11"/>
-      <c r="X6" s="11"/>
-      <c r="Y6" s="11"/>
-    </row>
-    <row r="7" spans="1:25">
+      <c r="Q6" s="3"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="6"/>
+      <c r="T6" s="6"/>
+      <c r="U6" s="6"/>
+      <c r="V6" s="6"/>
+      <c r="W6" s="6"/>
+      <c r="X6" s="6"/>
+      <c r="Y6" s="6"/>
+      <c r="Z6" s="6"/>
+      <c r="AA6" s="6"/>
+    </row>
+    <row r="7" spans="1:27">
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
-      <c r="P7" s="2" t="s">
+      <c r="O7" s="3"/>
+      <c r="P7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6"/>
+      <c r="T7" s="6"/>
+      <c r="U7" s="6"/>
+      <c r="V7" s="6"/>
+      <c r="W7" s="6"/>
+      <c r="X7" s="6"/>
+      <c r="Y7" s="6"/>
+      <c r="Z7" s="6"/>
+      <c r="AA7" s="6"/>
+    </row>
+    <row r="8" spans="1:27">
+      <c r="D8" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="R7" s="11"/>
-      <c r="S7" s="11"/>
-      <c r="T7" s="11"/>
-      <c r="U7" s="11"/>
-      <c r="V7" s="11"/>
-      <c r="W7" s="11"/>
-      <c r="X7" s="11"/>
-      <c r="Y7" s="11"/>
-    </row>
-    <row r="8" spans="1:25">
-      <c r="D8" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
+      <c r="O8" s="3"/>
       <c r="P8" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
-      <c r="R8" s="11"/>
-      <c r="S8" s="11"/>
-      <c r="T8" s="11"/>
-      <c r="U8" s="11"/>
-      <c r="V8" s="11"/>
-      <c r="W8" s="11"/>
-      <c r="X8" s="11"/>
-      <c r="Y8" s="11"/>
-    </row>
-    <row r="9" spans="1:25">
+      <c r="Q8" s="3"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="6"/>
+      <c r="U8" s="6"/>
+      <c r="V8" s="6"/>
+      <c r="W8" s="6"/>
+      <c r="X8" s="6"/>
+      <c r="Y8" s="6"/>
+      <c r="Z8" s="6"/>
+      <c r="AA8" s="6"/>
+    </row>
+    <row r="9" spans="1:27">
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
+      <c r="O9" s="3"/>
       <c r="P9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="6"/>
+      <c r="U9" s="6"/>
+      <c r="V9" s="6"/>
+      <c r="W9" s="6"/>
+      <c r="X9" s="6"/>
+      <c r="Y9" s="6"/>
+      <c r="Z9" s="6"/>
+      <c r="AA9" s="6"/>
+    </row>
+    <row r="10" spans="1:27">
+      <c r="D10" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="R9" s="11"/>
-      <c r="S9" s="11"/>
-      <c r="T9" s="11"/>
-      <c r="U9" s="11"/>
-      <c r="V9" s="11"/>
-      <c r="W9" s="11"/>
-      <c r="X9" s="11"/>
-      <c r="Y9" s="11"/>
-    </row>
-    <row r="10" spans="1:25">
-      <c r="D10" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
+      <c r="O10" s="3"/>
       <c r="P10" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
-      <c r="R10" s="14"/>
-      <c r="S10" s="14"/>
-      <c r="T10" s="14"/>
-      <c r="U10" s="14"/>
-      <c r="V10" s="14"/>
-      <c r="W10" s="14"/>
-      <c r="X10" s="14"/>
-      <c r="Y10" s="14"/>
-    </row>
-    <row r="11" spans="1:25">
+      <c r="Q10" s="3"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="6"/>
+      <c r="U10" s="6"/>
+      <c r="V10" s="6"/>
+      <c r="W10" s="6"/>
+      <c r="X10" s="6"/>
+      <c r="Y10" s="6"/>
+      <c r="Z10" s="6"/>
+      <c r="AA10" s="6"/>
+    </row>
+    <row r="11" spans="1:27">
+      <c r="D11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
-      <c r="R11" s="12"/>
-      <c r="S11" s="12"/>
-      <c r="T11" s="12"/>
-      <c r="U11" s="12"/>
-      <c r="V11" s="12"/>
-      <c r="W11" s="12"/>
-      <c r="X11" s="12"/>
-      <c r="Y11" s="12"/>
-    </row>
-    <row r="12" spans="1:25">
-      <c r="D12" s="1" t="s">
+      <c r="O11" s="3"/>
+      <c r="P11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="6"/>
+      <c r="T11" s="6"/>
+      <c r="U11" s="6"/>
+      <c r="V11" s="6"/>
+      <c r="W11" s="6"/>
+      <c r="X11" s="6"/>
+      <c r="Y11" s="6"/>
+      <c r="Z11" s="6"/>
+      <c r="AA11" s="6"/>
+    </row>
+    <row r="12" spans="1:27">
+      <c r="D12" s="16" t="s">
         <v>6</v>
       </c>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
-      <c r="R12" s="12"/>
-      <c r="S12" s="12"/>
-      <c r="T12" s="12"/>
-      <c r="U12" s="12"/>
-      <c r="V12" s="12"/>
-      <c r="W12" s="12"/>
-      <c r="X12" s="12"/>
-      <c r="Y12" s="12"/>
-    </row>
-    <row r="13" spans="1:25">
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="4"/>
+      <c r="S12" s="4"/>
+      <c r="T12" s="4"/>
+      <c r="U12" s="4"/>
+      <c r="V12" s="4"/>
+      <c r="W12" s="4"/>
+      <c r="X12" s="4"/>
+      <c r="Y12" s="4"/>
+      <c r="Z12" s="4"/>
+      <c r="AA12" s="4"/>
+    </row>
+    <row r="13" spans="1:27">
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
-      <c r="O13" s="1" t="s">
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="4"/>
+      <c r="S13" s="4"/>
+      <c r="T13" s="4"/>
+      <c r="U13" s="4"/>
+      <c r="V13" s="4"/>
+      <c r="W13" s="4"/>
+      <c r="X13" s="4"/>
+      <c r="Y13" s="4"/>
+      <c r="Z13" s="4"/>
+      <c r="AA13" s="4"/>
+    </row>
+    <row r="14" spans="1:27">
+      <c r="D14" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="R13" s="12"/>
-      <c r="S13" s="12"/>
-      <c r="T13" s="12"/>
-      <c r="U13" s="12"/>
-      <c r="V13" s="12"/>
-      <c r="W13" s="12"/>
-      <c r="X13" s="12"/>
-      <c r="Y13" s="12"/>
-    </row>
-    <row r="14" spans="1:25">
-      <c r="D14" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14" s="4"/>
+      <c r="E14" s="9"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
-      <c r="P14" s="1" t="s">
-        <v>5</v>
+      <c r="O14" s="5" t="s">
+        <v>12</v>
       </c>
-      <c r="R14" s="14"/>
-      <c r="S14" s="14"/>
-      <c r="T14" s="14"/>
-      <c r="U14" s="14"/>
-      <c r="V14" s="14"/>
-      <c r="W14" s="14"/>
-      <c r="X14" s="14"/>
-      <c r="Y14" s="14"/>
-    </row>
-    <row r="15" spans="1:25">
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="4"/>
+      <c r="S14" s="4"/>
+      <c r="T14" s="4"/>
+      <c r="U14" s="4"/>
+      <c r="V14" s="4"/>
+      <c r="W14" s="4"/>
+      <c r="X14" s="4"/>
+      <c r="Y14" s="4"/>
+      <c r="Z14" s="4"/>
+      <c r="AA14" s="4"/>
+    </row>
+    <row r="15" spans="1:27">
+      <c r="D15" s="17"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
+      <c r="O15" s="3"/>
       <c r="P15" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
-      <c r="R15" s="13"/>
-      <c r="S15" s="13"/>
-      <c r="T15" s="13"/>
-      <c r="U15" s="13"/>
-      <c r="V15" s="13"/>
-      <c r="W15" s="13"/>
-      <c r="X15" s="13"/>
-      <c r="Y15" s="13"/>
-    </row>
-    <row r="16" spans="1:25">
+      <c r="Q15" s="3"/>
+      <c r="R15" s="6"/>
+      <c r="S15" s="6"/>
+      <c r="T15" s="6"/>
+      <c r="U15" s="6"/>
+      <c r="V15" s="6"/>
+      <c r="W15" s="6"/>
+      <c r="X15" s="6"/>
+      <c r="Y15" s="6"/>
+      <c r="Z15" s="6"/>
+      <c r="AA15" s="6"/>
+    </row>
+    <row r="16" spans="1:27">
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
-      <c r="P16" s="2" t="s">
-        <v>7</v>
+      <c r="O16" s="3"/>
+      <c r="P16" s="1" t="s">
+        <v>6</v>
       </c>
-      <c r="R16" s="13"/>
-      <c r="S16" s="13"/>
-      <c r="T16" s="13"/>
-      <c r="U16" s="13"/>
-      <c r="V16" s="13"/>
-      <c r="W16" s="13"/>
-      <c r="X16" s="13"/>
-      <c r="Y16" s="13"/>
-    </row>
-    <row r="17" spans="4:25">
+      <c r="Q16" s="3"/>
+      <c r="R16" s="6"/>
+      <c r="S16" s="6"/>
+      <c r="T16" s="6"/>
+      <c r="U16" s="6"/>
+      <c r="V16" s="6"/>
+      <c r="W16" s="6"/>
+      <c r="X16" s="6"/>
+      <c r="Y16" s="6"/>
+      <c r="Z16" s="6"/>
+      <c r="AA16" s="6"/>
+    </row>
+    <row r="17" spans="4:27">
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
+      <c r="O17" s="3"/>
       <c r="P17" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
-      <c r="R17" s="13"/>
-      <c r="S17" s="13"/>
-      <c r="T17" s="13"/>
-      <c r="U17" s="13"/>
-      <c r="V17" s="13"/>
-      <c r="W17" s="13"/>
-      <c r="X17" s="13"/>
-      <c r="Y17" s="13"/>
-    </row>
-    <row r="18" spans="4:25">
+      <c r="Q17" s="3"/>
+      <c r="R17" s="6"/>
+      <c r="S17" s="6"/>
+      <c r="T17" s="6"/>
+      <c r="U17" s="6"/>
+      <c r="V17" s="6"/>
+      <c r="W17" s="6"/>
+      <c r="X17" s="6"/>
+      <c r="Y17" s="6"/>
+      <c r="Z17" s="6"/>
+      <c r="AA17" s="6"/>
+    </row>
+    <row r="18" spans="4:27">
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
+      <c r="O18" s="3"/>
       <c r="P18" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
-      <c r="R18" s="13"/>
-      <c r="S18" s="13"/>
-      <c r="T18" s="13"/>
-      <c r="U18" s="13"/>
-      <c r="V18" s="13"/>
-      <c r="W18" s="13"/>
-      <c r="X18" s="13"/>
-      <c r="Y18" s="13"/>
-    </row>
-    <row r="19" spans="4:25">
-      <c r="D19" s="7"/>
-      <c r="E19" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G19" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="H19" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="I19" s="8" t="s">
-        <v>19</v>
-      </c>
+      <c r="Q18" s="3"/>
+      <c r="R18" s="6"/>
+      <c r="S18" s="6"/>
+      <c r="T18" s="6"/>
+      <c r="U18" s="6"/>
+      <c r="V18" s="6"/>
+      <c r="W18" s="6"/>
+      <c r="X18" s="6"/>
+      <c r="Y18" s="6"/>
+      <c r="Z18" s="6"/>
+      <c r="AA18" s="6"/>
+    </row>
+    <row r="19" spans="4:27">
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
+      <c r="O19" s="3"/>
       <c r="P19" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
-      <c r="R19" s="13"/>
-      <c r="S19" s="13"/>
-      <c r="T19" s="13"/>
-      <c r="U19" s="13"/>
-      <c r="V19" s="13"/>
-      <c r="W19" s="13"/>
-      <c r="X19" s="13"/>
-      <c r="Y19" s="13"/>
-    </row>
-    <row r="20" spans="4:25">
-      <c r="D20" s="9" t="s">
-        <v>30</v>
+      <c r="Q19" s="3"/>
+      <c r="R19" s="6"/>
+      <c r="S19" s="6"/>
+      <c r="T19" s="6"/>
+      <c r="U19" s="6"/>
+      <c r="V19" s="6"/>
+      <c r="W19" s="6"/>
+      <c r="X19" s="6"/>
+      <c r="Y19" s="6"/>
+      <c r="Z19" s="6"/>
+      <c r="AA19" s="6"/>
+    </row>
+    <row r="20" spans="4:27">
+      <c r="D20" s="11"/>
+      <c r="E20" s="14" t="s">
+        <v>14</v>
       </c>
-      <c r="E20" s="8">
-        <v>100</v>
+      <c r="F20" s="14" t="s">
+        <v>15</v>
       </c>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7">
-        <f t="shared" ref="I20:I25" si="0">SUM(E20, F20, G20, H20)</f>
-        <v>100</v>
+      <c r="G20" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H20" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="I20" s="14" t="s">
+        <v>18</v>
       </c>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
-    </row>
-    <row r="21" spans="4:25">
-      <c r="D21" s="10" t="s">
-        <v>20</v>
+      <c r="O20" s="3"/>
+      <c r="P20" s="1" t="s">
+        <v>11</v>
       </c>
-      <c r="E21" s="8">
-        <v>5</v>
+      <c r="Q20" s="3"/>
+      <c r="R20" s="6"/>
+      <c r="S20" s="6"/>
+      <c r="T20" s="6"/>
+      <c r="U20" s="6"/>
+      <c r="V20" s="6"/>
+      <c r="W20" s="6"/>
+      <c r="X20" s="6"/>
+      <c r="Y20" s="6"/>
+      <c r="Z20" s="6"/>
+      <c r="AA20" s="6"/>
+    </row>
+    <row r="21" spans="4:27">
+      <c r="D21" s="15" t="s">
+        <v>29</v>
       </c>
-      <c r="F21" s="8"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7">
-        <f t="shared" si="0"/>
-        <v>5</v>
+      <c r="E21" s="12">
+        <v>100</v>
+      </c>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11">
+        <f t="shared" ref="I21:I26" si="0">SUM(E21, F21, G21, H21)</f>
+        <v>100</v>
       </c>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
-      <c r="O21" s="1" t="s">
-        <v>21</v>
+      <c r="O21" s="3"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
+      <c r="R21" s="3"/>
+      <c r="S21" s="3"/>
+      <c r="T21" s="3"/>
+      <c r="U21" s="3"/>
+      <c r="V21" s="3"/>
+      <c r="W21" s="3"/>
+      <c r="X21" s="3"/>
+      <c r="Y21" s="3"/>
+      <c r="Z21" s="3"/>
+      <c r="AA21" s="3"/>
+    </row>
+    <row r="22" spans="4:27">
+      <c r="D22" s="13" t="s">
+        <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="4:25">
-      <c r="D22" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E22" s="8">
+      <c r="E22" s="12">
         <v>5</v>
       </c>
-      <c r="F22" s="8"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7">
+      <c r="F22" s="12"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
-    </row>
-    <row r="23" spans="4:25">
-      <c r="D23" s="10" t="s">
-        <v>23</v>
+      <c r="O22" s="5" t="s">
+        <v>28</v>
       </c>
-      <c r="E23" s="8">
+      <c r="P22" s="5"/>
+      <c r="Q22" s="5"/>
+      <c r="R22" s="3"/>
+      <c r="S22" s="3"/>
+      <c r="T22" s="3"/>
+      <c r="U22" s="3"/>
+      <c r="V22" s="3"/>
+      <c r="W22" s="3"/>
+      <c r="X22" s="3"/>
+      <c r="Y22" s="3"/>
+      <c r="Z22" s="3"/>
+      <c r="AA22" s="3"/>
+    </row>
+    <row r="23" spans="4:27">
+      <c r="D23" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E23" s="12">
         <v>5</v>
       </c>
-      <c r="F23" s="8"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7">
+      <c r="F23" s="12"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
-    </row>
-    <row r="24" spans="4:25">
-      <c r="D24" s="10" t="s">
-        <v>24</v>
+      <c r="O23" s="3"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="3"/>
+      <c r="R23" s="3"/>
+      <c r="S23" s="3"/>
+      <c r="T23" s="3"/>
+      <c r="U23" s="3"/>
+      <c r="V23" s="3"/>
+      <c r="W23" s="3"/>
+      <c r="X23" s="3"/>
+      <c r="Y23" s="3"/>
+      <c r="Z23" s="3"/>
+      <c r="AA23" s="3"/>
+    </row>
+    <row r="24" spans="4:27">
+      <c r="D24" s="13" t="s">
+        <v>21</v>
       </c>
-      <c r="E24" s="8">
+      <c r="E24" s="12">
         <v>5</v>
       </c>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="7">
+      <c r="F24" s="12"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
-    </row>
-    <row r="25" spans="4:25">
-      <c r="D25" s="10" t="s">
-        <v>25</v>
+      <c r="O24" s="3"/>
+      <c r="P24" s="3"/>
+      <c r="Q24" s="3"/>
+      <c r="R24" s="3"/>
+      <c r="S24" s="3"/>
+      <c r="T24" s="3"/>
+      <c r="U24" s="3"/>
+      <c r="V24" s="3"/>
+      <c r="W24" s="3"/>
+      <c r="X24" s="3"/>
+      <c r="Y24" s="3"/>
+      <c r="Z24" s="3"/>
+      <c r="AA24" s="3"/>
+    </row>
+    <row r="25" spans="4:27">
+      <c r="D25" s="13" t="s">
+        <v>22</v>
       </c>
-      <c r="E25" s="8">
+      <c r="E25" s="12">
         <v>5</v>
       </c>
-      <c r="F25" s="8"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7">
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="11">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
-    </row>
-    <row r="26" spans="4:25">
+      <c r="O25" s="3"/>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="3"/>
+      <c r="R25" s="3"/>
+      <c r="S25" s="3"/>
+      <c r="T25" s="3"/>
+      <c r="U25" s="3"/>
+      <c r="V25" s="3"/>
+      <c r="W25" s="3"/>
+      <c r="X25" s="3"/>
+      <c r="Y25" s="3"/>
+      <c r="Z25" s="3"/>
+      <c r="AA25" s="3"/>
+    </row>
+    <row r="26" spans="4:27">
+      <c r="D26" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E26" s="12">
+        <v>5</v>
+      </c>
+      <c r="F26" s="12"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
-    </row>
-    <row r="27" spans="4:25">
-      <c r="D27" s="1" t="s">
-        <v>26</v>
-      </c>
+      <c r="O26" s="3"/>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="3"/>
+      <c r="R26" s="3"/>
+      <c r="S26" s="3"/>
+      <c r="T26" s="3"/>
+      <c r="U26" s="3"/>
+      <c r="V26" s="3"/>
+      <c r="W26" s="3"/>
+      <c r="X26" s="3"/>
+      <c r="Y26" s="3"/>
+      <c r="Z26" s="3"/>
+      <c r="AA26" s="3"/>
+    </row>
+    <row r="27" spans="4:27">
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
-    </row>
-    <row r="28" spans="4:25">
+      <c r="O27" s="3"/>
+      <c r="P27" s="3"/>
+      <c r="Q27" s="3"/>
+      <c r="R27" s="3"/>
+      <c r="S27" s="3"/>
+      <c r="T27" s="3"/>
+      <c r="U27" s="3"/>
+      <c r="V27" s="3"/>
+      <c r="W27" s="3"/>
+      <c r="X27" s="3"/>
+      <c r="Y27" s="3"/>
+      <c r="Z27" s="3"/>
+      <c r="AA27" s="3"/>
+    </row>
+    <row r="28" spans="4:27">
+      <c r="D28" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
-      <c r="O28" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="4:25">
-      <c r="D29" s="1" t="s">
-        <v>28</v>
-      </c>
+      <c r="O28" s="3"/>
+      <c r="P28" s="3"/>
+      <c r="Q28" s="3"/>
+      <c r="R28" s="3"/>
+      <c r="S28" s="3"/>
+      <c r="T28" s="3"/>
+      <c r="U28" s="3"/>
+      <c r="V28" s="3"/>
+      <c r="W28" s="3"/>
+      <c r="X28" s="3"/>
+      <c r="Y28" s="3"/>
+      <c r="Z28" s="3"/>
+      <c r="AA28" s="3"/>
+    </row>
+    <row r="29" spans="4:27">
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
-    </row>
-    <row r="30" spans="4:25">
+      <c r="O29" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="P29" s="3"/>
+      <c r="Q29" s="3"/>
+      <c r="R29" s="3"/>
+      <c r="S29" s="3"/>
+      <c r="T29" s="3"/>
+      <c r="U29" s="3"/>
+      <c r="V29" s="3"/>
+      <c r="W29" s="3"/>
+      <c r="X29" s="3"/>
+      <c r="Y29" s="3"/>
+      <c r="Z29" s="3"/>
+      <c r="AA29" s="3"/>
+    </row>
+    <row r="30" spans="4:27">
+      <c r="D30" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
     </row>
-    <row r="31" spans="4:25">
+    <row r="31" spans="4:27">
+      <c r="D31" s="2"/>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
     </row>
-    <row r="32" spans="4:25">
-      <c r="D32" s="1" t="s">
-        <v>29</v>
-      </c>
+    <row r="32" spans="4:27">
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
     </row>
-    <row r="33" spans="11:13">
+    <row r="33" spans="4:13">
+      <c r="D33" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
     </row>
-    <row r="34" spans="11:13">
+    <row r="34" spans="4:13">
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
     </row>
-    <row r="35" spans="11:13">
+    <row r="35" spans="4:13">
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
     </row>
-    <row r="36" spans="11:13">
+    <row r="36" spans="4:13">
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
     </row>
-    <row r="37" spans="11:13">
+    <row r="37" spans="4:13">
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
     </row>
-    <row r="38" spans="11:13">
+    <row r="38" spans="4:13">
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
     </row>
-    <row r="39" spans="11:13">
+    <row r="39" spans="4:13">
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
     </row>
-    <row r="40" spans="11:13">
+    <row r="40" spans="4:13">
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
       <c r="M40" s="1"/>
     </row>
-    <row r="41" spans="11:13">
+    <row r="41" spans="4:13">
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
       <c r="M41" s="1"/>
     </row>
-    <row r="42" spans="11:13">
+    <row r="42" spans="4:13">
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
       <c r="M42" s="1"/>
     </row>
-    <row r="43" spans="11:13">
+    <row r="43" spans="4:13">
       <c r="K43" s="1"/>
       <c r="L43" s="1"/>
       <c r="M43" s="1"/>
     </row>
-    <row r="44" spans="11:13">
+    <row r="44" spans="4:13">
       <c r="K44" s="1"/>
       <c r="L44" s="1"/>
       <c r="M44" s="1"/>
     </row>
-    <row r="45" spans="11:13">
+    <row r="45" spans="4:13">
       <c r="K45" s="1"/>
       <c r="L45" s="1"/>
       <c r="M45" s="1"/>
     </row>
-    <row r="46" spans="11:13">
+    <row r="46" spans="4:13">
       <c r="K46" s="1"/>
       <c r="L46" s="1"/>
       <c r="M46" s="1"/>
     </row>
-    <row r="47" spans="11:13">
+    <row r="47" spans="4:13">
       <c r="K47" s="1"/>
       <c r="L47" s="1"/>
       <c r="M47" s="1"/>
     </row>
-    <row r="48" spans="11:13">
+    <row r="48" spans="4:13">
       <c r="K48" s="1"/>
       <c r="L48" s="1"/>
       <c r="M48" s="1"/>
@@ -5850,12 +6067,30 @@
       <c r="M1000" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="D2:H3"/>
+  <mergeCells count="20">
     <mergeCell ref="O2:P3"/>
     <mergeCell ref="D14:E14"/>
+    <mergeCell ref="E4:H4"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="E8:H8"/>
+    <mergeCell ref="E10:H10"/>
+    <mergeCell ref="E12:H12"/>
+    <mergeCell ref="D2:H3"/>
+    <mergeCell ref="R20:AA20"/>
+    <mergeCell ref="R6:AA6"/>
+    <mergeCell ref="R7:AA7"/>
+    <mergeCell ref="R8:AA8"/>
+    <mergeCell ref="R9:AA9"/>
+    <mergeCell ref="R10:AA10"/>
+    <mergeCell ref="R11:AA11"/>
+    <mergeCell ref="R15:AA15"/>
+    <mergeCell ref="R16:AA16"/>
+    <mergeCell ref="R17:AA17"/>
+    <mergeCell ref="R18:AA18"/>
+    <mergeCell ref="R19:AA19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>